<commit_message>
negative control tests work. Reference directory updated
</commit_message>
<xml_diff>
--- a/test/negative_control/out/KCOR_summary.xlsx
+++ b/test/negative_control/out/KCOR_summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,17 +481,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9723</t>
+          <t>1.0496</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>1.023</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.077</t>
         </is>
       </c>
     </row>
@@ -499,159 +499,228 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9723</t>
+          <t>1.1032</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.9963</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.958</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.036</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2 vs 0</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.0541</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.996</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1.115</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>ASMR (pooled)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0541</t>
+          <t>1.1473</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.185</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1.2507</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1.192</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1.313</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2 vs 1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.0481</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1.005</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1.093</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.0841</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1.027</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1.144</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1.0841</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1.027</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1.144</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.0931</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1.059</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1.129</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1.1337</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1.079</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1.191</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1.0521</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1.011</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1.095</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -664,7 +733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,17 +788,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0261</t>
+          <t>0.9996</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.971</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -737,159 +806,228 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0261</t>
+          <t>0.9929</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.035</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.0063</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.967</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.047</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2 vs 0</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.0493</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.989</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1.113</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>ASMR (pooled)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0493</t>
+          <t>1.0941</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>1.058</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.131</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1.1580</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1.102</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1.217</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2 vs 1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.0349</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.990</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1.082</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.0496</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.989</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1.114</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1.0496</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.989</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1.114</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.1407</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1.104</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1.178</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1.2430</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1.185</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1.304</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1.0488</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1.003</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1.096</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated readme and negative control test
</commit_message>
<xml_diff>
--- a/test/negative_control/out/KCOR_summary.xlsx
+++ b/test/negative_control/out/KCOR_summary.xlsx
@@ -481,17 +481,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0287</t>
+          <t>1.0097</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>0.992</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.027</t>
         </is>
       </c>
     </row>
@@ -527,17 +527,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9963</t>
+          <t>0.9330</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.898</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -550,17 +550,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0115</t>
+          <t>1.0041</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.981</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.028</t>
         </is>
       </c>
     </row>
@@ -591,17 +591,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0798</t>
+          <t>1.0213</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.103</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
@@ -637,17 +637,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0481</t>
+          <t>0.8769</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>0.914</t>
         </is>
       </c>
     </row>
@@ -660,17 +660,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0263</t>
+          <t>0.9967</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>0.970</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.024</t>
         </is>
       </c>
     </row>
@@ -701,17 +701,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.0496</t>
+          <t>1.0115</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.991</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.033</t>
         </is>
       </c>
     </row>
@@ -747,17 +747,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0521</t>
+          <t>0.9398</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>0.903</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>0.978</t>
         </is>
       </c>
     </row>
@@ -770,17 +770,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0146</t>
+          <t>0.9926</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.020</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0000</t>
+          <t>0.9858</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.970</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.002</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9929</t>
+          <t>0.9316</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>0.971</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0063</t>
+          <t>0.9868</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.967</t>
+          <t>0.948</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.027</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
should be VERY close now
</commit_message>
<xml_diff>
--- a/test/negative_control/out/KCOR_summary.xlsx
+++ b/test/negative_control/out/KCOR_summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1 vs 0</t>
+          <t>Reporting date: 2023-01-02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -473,48 +473,36 @@
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1.0097</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.992</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1.027</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1 vs 0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1940</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1032</t>
+          <t>0.9962</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -522,22 +510,22 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>All Ages</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9330</t>
+          <t>0.9844</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.898</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.994</t>
         </is>
       </c>
     </row>
@@ -545,109 +533,109 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0041</t>
+          <t>1.0683</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.981</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.088</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.9669</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.945</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.990</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2 vs 0</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.9834</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.970</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.997</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1.0213</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1.000</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.043</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.2507</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.192</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1.313</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8769</t>
+          <t>1.0244</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>1.013</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>1.036</t>
         </is>
       </c>
     </row>
@@ -655,141 +643,233 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>All Ages</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9967</t>
+          <t>1.0003</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>1.012</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.2383</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1.208</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1.269</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2 vs 1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.9163</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.894</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0.939</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ASMR (pooled)</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.0115</t>
+          <t>1.0036</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.988</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.019</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1.1337</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1.079</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>1.191</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0.9398</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.903</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0.978</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.9926</t>
+          <t>1.0283</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>1.017</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1.0161</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1.005</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1.028</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1.1591</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1.131</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1.188</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.9477</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.925</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.971</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1.0205</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1.005</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1.036</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -802,7 +882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,7 +920,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1 vs 0</t>
+          <t>Reporting date: 2023-01-02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -849,48 +929,36 @@
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.9858</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.970</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1.002</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1 vs 0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1940</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9316</t>
+          <t>1.0093</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>0.993</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>1.025</t>
         </is>
       </c>
     </row>
@@ -898,22 +966,22 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>All Ages</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9868</t>
+          <t>1.0044</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.948</t>
+          <t>0.988</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -921,109 +989,109 @@
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>1940</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0002</t>
+          <t>1.0056</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.053</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.9922</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.953</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1.033</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2 vs 0</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.0159</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.997</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.035</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1.0756</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>1.055</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.097</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.1580</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.102</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1.217</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0349</t>
+          <t>1.0338</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.052</t>
         </is>
       </c>
     </row>
@@ -1031,141 +1099,233 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>All Ages</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0660</t>
+          <t>1.0279</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1.0949</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1.042</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1.151</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2 vs 1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1.0267</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.983</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1.073</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ASMR (pooled)</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.0911</t>
+          <t>1.0207</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.070</t>
+          <t>0.999</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1.2430</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1.185</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>1.304</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1.0488</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>1.003</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1.096</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>ASMR (direct)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0657</t>
+          <t>1.0243</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.042</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1.0234</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1.005</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1.042</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1.0888</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1.038</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1.142</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1.0348</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.991</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1.081</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1.0047</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.983</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1.027</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>